<commit_message>
yeni uygulama enginne,api,service , ticket_simple
</commit_message>
<xml_diff>
--- a/ticket_tahminleri_new.xlsx
+++ b/ticket_tahminleri_new.xlsx
@@ -140,1612 +140,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Ankara Aylık Ticket Tahminleri</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Ankara'!B1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Ankara'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Ankara'!$C$1:$J$1</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'Ankara'!B2</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Ankara'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Ankara'!$C$2:$J$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'Ankara'!B3</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Ankara'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Ankara'!$C$3:$J$3</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <strRef>
-              <f>'Ankara'!B4</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Ankara'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Ankara'!$C$4:$J$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <strRef>
-              <f>'Ankara'!B5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Ankara'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Ankara'!$C$5:$J$5</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </lineChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Aylar</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Ticket Sayısı</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Antalya Aylık Ticket Tahminleri</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Antalya'!B1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Antalya'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Antalya'!$C$1:$J$1</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'Antalya'!B2</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Antalya'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Antalya'!$C$2:$J$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'Antalya'!B3</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Antalya'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Antalya'!$C$3:$J$3</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <strRef>
-              <f>'Antalya'!B4</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Antalya'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Antalya'!$C$4:$J$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </lineChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Aylar</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Ticket Sayısı</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Bursa Aylık Ticket Tahminleri</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Bursa'!B1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Bursa'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Bursa'!$C$1:$J$1</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'Bursa'!B2</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Bursa'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Bursa'!$C$2:$J$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'Bursa'!B3</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Bursa'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Bursa'!$C$3:$J$3</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <strRef>
-              <f>'Bursa'!B4</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'Bursa'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Bursa'!$C$4:$J$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </lineChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Aylar</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Ticket Sayısı</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>İstanbul-Anadolu Aylık Ticket Tahminleri</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Anadolu'!B1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Anadolu'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Anadolu'!$C$1:$J$1</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Anadolu'!B2</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Anadolu'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Anadolu'!$C$2:$J$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Anadolu'!B3</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Anadolu'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Anadolu'!$C$3:$J$3</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Anadolu'!B4</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Anadolu'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Anadolu'!$C$4:$J$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Anadolu'!B5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Anadolu'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Anadolu'!$C$5:$J$5</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </lineChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Aylar</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Ticket Sayısı</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>İstanbul-Avrupa Aylık Ticket Tahminleri</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Avrupa'!B1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$C$1:$J$1</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Avrupa'!B2</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$C$2:$J$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Avrupa'!B3</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$C$3:$J$3</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Avrupa'!B4</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$C$4:$J$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Avrupa'!B5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$C$5:$J$5</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <strRef>
-              <f>'İstanbul-Avrupa'!B6</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İstanbul-Avrupa'!$C$6:$J$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </lineChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Aylar</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Ticket Sayısı</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>İzmir Aylık Ticket Tahminleri</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <lineChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'İzmir'!B1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İzmir'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İzmir'!$C$1:$J$1</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'İzmir'!B2</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İzmir'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İzmir'!$C$2:$J$2</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'İzmir'!B3</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İzmir'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İzmir'!$C$3:$J$3</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <strRef>
-              <f>'İzmir'!B4</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İzmir'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İzmir'!$C$4:$J$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <strRef>
-              <f>'İzmir'!B5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <cat>
-            <numRef>
-              <f>'İzmir'!$B$1:$J$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'İzmir'!$C$5:$J$5</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </lineChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Aylar</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Ticket Sayısı</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>8</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>7</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>7</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>8</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>9</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>8</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2303,7 +697,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2542,7 +935,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2781,7 +1173,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3057,7 +1448,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3370,7 +1760,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3646,6 +2035,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>